<commit_message>
entered tree species latin names with the exception of sporadic illegible species names
</commit_message>
<xml_diff>
--- a/Lovejoy_data_table_tree_frequency.xlsx
+++ b/Lovejoy_data_table_tree_frequency.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
   <si>
     <t>Treespecies</t>
   </si>
@@ -33,6 +33,411 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Allantoma Lineata</t>
+  </si>
+  <si>
+    <t>Anacardium Giganteum</t>
+  </si>
+  <si>
+    <t>Andira Retusa</t>
+  </si>
+  <si>
+    <t>Aniba Burchellii</t>
+  </si>
+  <si>
+    <t>Aparisthmium Cordatum</t>
+  </si>
+  <si>
+    <t>Apeiba Burchellii</t>
+  </si>
+  <si>
+    <t>Apeiba sp.</t>
+  </si>
+  <si>
+    <t>Arrabidea Tuberculata</t>
+  </si>
+  <si>
+    <t>Aspidosperma Verruculosum</t>
+  </si>
+  <si>
+    <t>Asoidosperma sp.</t>
+  </si>
+  <si>
+    <t>Caraipa Grandiflora</t>
+  </si>
+  <si>
+    <t>Carapa Guianensis</t>
+  </si>
+  <si>
+    <t>Caryocar Glabrum</t>
+  </si>
+  <si>
+    <t>Cassipourea Guianensis</t>
+  </si>
+  <si>
+    <t>Cecropia Juranyiana</t>
+  </si>
+  <si>
+    <t>Cecropia Obtusa</t>
+  </si>
+  <si>
+    <t>Cecropia sp.</t>
+  </si>
+  <si>
+    <t>Ceiba Pentandra</t>
+  </si>
+  <si>
+    <t>Cheiloclinium Cognatum</t>
+  </si>
+  <si>
+    <t>Chimarrhis Turbinata</t>
+  </si>
+  <si>
+    <t>Chrysophyllum Prieurei</t>
+  </si>
+  <si>
+    <t>Chrysophyllum sp.</t>
+  </si>
+  <si>
+    <t>Coccoloba Latifulia</t>
+  </si>
+  <si>
+    <t>Conceveiba Guianensis</t>
+  </si>
+  <si>
+    <t>Cordia Scabrida</t>
+  </si>
+  <si>
+    <t>Cordia Scabrifolia</t>
+  </si>
+  <si>
+    <t>Cordia sp.</t>
+  </si>
+  <si>
+    <t>Couepia Divaricata</t>
+  </si>
+  <si>
+    <t>Couepia Hoffmanniana</t>
+  </si>
+  <si>
+    <t>Couepia Leptostachya</t>
+  </si>
+  <si>
+    <t>Coumarouna Odorata</t>
+  </si>
+  <si>
+    <t>Coumarouna sp.</t>
+  </si>
+  <si>
+    <t>Couratari Pulchra</t>
+  </si>
+  <si>
+    <t>Coussapoa Trinervia</t>
+  </si>
+  <si>
+    <t>Crepisospermum sp.</t>
+  </si>
+  <si>
+    <t>Crudia Oblonga</t>
+  </si>
+  <si>
+    <t>Cupania sp.</t>
+  </si>
+  <si>
+    <t>Dacryodes Belemensis</t>
+  </si>
+  <si>
+    <t>Davilla Aspera</t>
+  </si>
+  <si>
+    <t>Dendrobangia Boliviana</t>
+  </si>
+  <si>
+    <t>Dialium Guianense</t>
+  </si>
+  <si>
+    <t>Didymopanax Morototoni</t>
+  </si>
+  <si>
+    <t>Diospyros Mellinoni</t>
+  </si>
+  <si>
+    <t>Emmotum Acuminatum</t>
+  </si>
+  <si>
+    <t>Emmotum Fagifolium</t>
+  </si>
+  <si>
+    <t>Erisma Uncinatum</t>
+  </si>
+  <si>
+    <t>Eschweilera Odora</t>
+  </si>
+  <si>
+    <t>Eschweilera Panicolata</t>
+  </si>
+  <si>
+    <t>Eschweilera sp. 1</t>
+  </si>
+  <si>
+    <t>Eschweilera sp. 2</t>
+  </si>
+  <si>
+    <t>Eschweilera sp. 3</t>
+  </si>
+  <si>
+    <t>Eschweilera sp. 4</t>
+  </si>
+  <si>
+    <t>Eugenia Correal</t>
+  </si>
+  <si>
+    <t>Eugenia Pairisii</t>
+  </si>
+  <si>
+    <t>Ficus sp.</t>
+  </si>
+  <si>
+    <t>Fusaea Longifolia</t>
+  </si>
+  <si>
+    <t>Goupia Glabra</t>
+  </si>
+  <si>
+    <t>Guatteria sp.</t>
+  </si>
+  <si>
+    <t>Gustavia Augusta</t>
+  </si>
+  <si>
+    <t>Gustavia sp.</t>
+  </si>
+  <si>
+    <t>Hebepetalum Humirifolium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heisteria sp. </t>
+  </si>
+  <si>
+    <t>Helicostylis Pedunculata</t>
+  </si>
+  <si>
+    <t>Helicostylis Tomentosa</t>
+  </si>
+  <si>
+    <t>Hevea Brasiliensis</t>
+  </si>
+  <si>
+    <t>Hippocrateaceae</t>
+  </si>
+  <si>
+    <t>Humiriastrum Excelsum</t>
+  </si>
+  <si>
+    <t>Hymenaea Oblongifolia</t>
+  </si>
+  <si>
+    <t>Hymenolobium Excelsum</t>
+  </si>
+  <si>
+    <t>Inga Auristellae</t>
+  </si>
+  <si>
+    <t>Inga Cayennensis</t>
+  </si>
+  <si>
+    <t>Inga Crassifolia</t>
+  </si>
+  <si>
+    <t>Lauraceae</t>
+  </si>
+  <si>
+    <t>Licania Latifolia</t>
+  </si>
+  <si>
+    <t>Licania Longistyla</t>
+  </si>
+  <si>
+    <t>Licania Macrophylla</t>
+  </si>
+  <si>
+    <t>Licania Micrantha</t>
+  </si>
+  <si>
+    <t>Licania sp.</t>
+  </si>
+  <si>
+    <t>Licaria Camara</t>
+  </si>
+  <si>
+    <t>Macrolobium Bifolium</t>
+  </si>
+  <si>
+    <t>Maprounea Guianensis</t>
+  </si>
+  <si>
+    <t>Micropholis Acutangula</t>
+  </si>
+  <si>
+    <t>Micropholis Calophylloides</t>
+  </si>
+  <si>
+    <t>Micropholis Eugeniifolia</t>
+  </si>
+  <si>
+    <t>Micropholis Guianensis</t>
+  </si>
+  <si>
+    <t>Mouriria Huberi</t>
+  </si>
+  <si>
+    <t>Mouriria Sagotiana</t>
+  </si>
+  <si>
+    <t>Myrcia sp.</t>
+  </si>
+  <si>
+    <t>Neea Glomeruliflora</t>
+  </si>
+  <si>
+    <t>Piptadenia Suaveolens</t>
+  </si>
+  <si>
+    <t>Pithacellobium Jupunba</t>
+  </si>
+  <si>
+    <t>Poraqueiba Guianensis</t>
+  </si>
+  <si>
+    <t>Pourouma Melinonii</t>
+  </si>
+  <si>
+    <t>Porouma Myrmecophila</t>
+  </si>
+  <si>
+    <t>Pourouma sp.</t>
+  </si>
+  <si>
+    <t>Pouteria Cladantha</t>
+  </si>
+  <si>
+    <t>Pouteria Guianensis</t>
+  </si>
+  <si>
+    <t>Pouteria Laurifolia</t>
+  </si>
+  <si>
+    <t>Pouteria App Paraensis</t>
+  </si>
+  <si>
+    <t>Pouteria Virescens</t>
+  </si>
+  <si>
+    <t>Pouteria sp.</t>
+  </si>
+  <si>
+    <t>Protium Aracouchini</t>
+  </si>
+  <si>
+    <t>Protium Cuneatum</t>
+  </si>
+  <si>
+    <t>Protium Decandrum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protium Guacayanum </t>
+  </si>
+  <si>
+    <t>Protium Neglectum</t>
+  </si>
+  <si>
+    <t>Protium Paraense</t>
+  </si>
+  <si>
+    <t>Protium Polybotryum</t>
+  </si>
+  <si>
+    <t>Protium Puncticulatum</t>
+  </si>
+  <si>
+    <t>Pterocarpus Amazonicus</t>
+  </si>
+  <si>
+    <t>Ptychopetalum Olacoides</t>
+  </si>
+  <si>
+    <t>Qualea Albiflora</t>
+  </si>
+  <si>
+    <t>Rheedia Macrophylla</t>
+  </si>
+  <si>
+    <t>Rinorea Flavescens</t>
+  </si>
+  <si>
+    <t>Rubiaceae</t>
+  </si>
+  <si>
+    <t>Sloanea Guianensis</t>
+  </si>
+  <si>
+    <t>Sterculia Pruriens</t>
+  </si>
+  <si>
+    <t>Sterculia sp.</t>
+  </si>
+  <si>
+    <t>Symphonia Globulifera</t>
+  </si>
+  <si>
+    <t>Tachigalia Myrmecophylla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tapura Singularis </t>
+  </si>
+  <si>
+    <t>Terminalia Amazonia</t>
+  </si>
+  <si>
+    <t>Tetragastris Altissima</t>
+  </si>
+  <si>
+    <t>Tetragastris Pilosa</t>
+  </si>
+  <si>
+    <t>Tetragastris Trifoliolata</t>
+  </si>
+  <si>
+    <t>Theobroma Speciosum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Theobroma Subincanum </t>
+  </si>
+  <si>
+    <t>Thyrsodium Paraensis</t>
+  </si>
+  <si>
+    <t>Tovomita Stigmatosa</t>
+  </si>
+  <si>
+    <t>Tovomita sp.</t>
+  </si>
+  <si>
+    <t>Vantanea Guianensis</t>
+  </si>
+  <si>
+    <t>Vantanea Parviflora</t>
+  </si>
+  <si>
+    <t>Vatairea Guianensis</t>
+  </si>
+  <si>
+    <t>Virola Surinamensis</t>
+  </si>
+  <si>
+    <t>Vochysia Guianensis</t>
   </si>
 </sst>
 </file>
@@ -352,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CB250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BH230" workbookViewId="0">
-      <selection activeCell="BA250" sqref="BA250"/>
+    <sheetView tabSelected="1" topLeftCell="A234" workbookViewId="0">
+      <selection activeCell="B162" sqref="B162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,6 +1009,9 @@
       <c r="A2">
         <v>4</v>
       </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
       <c r="C2">
         <v>66</v>
       </c>
@@ -843,6 +1251,9 @@
       <c r="A3">
         <v>7</v>
       </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
       <c r="C3">
         <v>25</v>
       </c>
@@ -1082,6 +1493,9 @@
       <c r="A4">
         <v>8</v>
       </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
       <c r="C4">
         <v>14</v>
       </c>
@@ -1321,6 +1735,9 @@
       <c r="A5">
         <v>9</v>
       </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
       <c r="C5">
         <v>12</v>
       </c>
@@ -1560,6 +1977,9 @@
       <c r="A6">
         <v>11</v>
       </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
       <c r="C6">
         <v>5</v>
       </c>
@@ -1799,6 +2219,9 @@
       <c r="A7">
         <v>12</v>
       </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
       <c r="C7">
         <v>65</v>
       </c>
@@ -2038,6 +2461,9 @@
       <c r="A8">
         <v>14</v>
       </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
       <c r="C8">
         <v>28</v>
       </c>
@@ -2277,6 +2703,9 @@
       <c r="A9">
         <v>15</v>
       </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
       <c r="C9">
         <v>7</v>
       </c>
@@ -2516,6 +2945,9 @@
       <c r="A10">
         <v>17</v>
       </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
       <c r="C10">
         <v>5</v>
       </c>
@@ -2755,6 +3187,9 @@
       <c r="A11">
         <v>18</v>
       </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
       <c r="C11">
         <v>5</v>
       </c>
@@ -2994,6 +3429,9 @@
       <c r="A12">
         <v>28</v>
       </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
       <c r="C12">
         <v>130</v>
       </c>
@@ -3233,6 +3671,9 @@
       <c r="A13">
         <v>29</v>
       </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
       <c r="C13">
         <v>104</v>
       </c>
@@ -3472,6 +3913,9 @@
       <c r="A14">
         <v>30</v>
       </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
       <c r="C14">
         <v>19</v>
       </c>
@@ -3711,6 +4155,9 @@
       <c r="A15">
         <v>32</v>
       </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
       <c r="C15">
         <v>90</v>
       </c>
@@ -3950,6 +4397,9 @@
       <c r="A16">
         <v>33</v>
       </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
       <c r="C16">
         <v>70</v>
       </c>
@@ -4189,6 +4639,9 @@
       <c r="A17">
         <v>34</v>
       </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
       <c r="C17">
         <v>51</v>
       </c>
@@ -4428,6 +4881,9 @@
       <c r="A18">
         <v>35</v>
       </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
       <c r="C18">
         <v>110</v>
       </c>
@@ -4667,6 +5123,9 @@
       <c r="A19">
         <v>36</v>
       </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
       <c r="C19">
         <v>82</v>
       </c>
@@ -4906,6 +5365,9 @@
       <c r="A20">
         <v>37</v>
       </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
       <c r="C20">
         <v>71</v>
       </c>
@@ -5145,6 +5607,9 @@
       <c r="A21">
         <v>38</v>
       </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
       <c r="C21">
         <v>67</v>
       </c>
@@ -5384,6 +5849,9 @@
       <c r="A22">
         <v>39</v>
       </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
       <c r="C22">
         <v>57</v>
       </c>
@@ -5623,6 +6091,9 @@
       <c r="A23">
         <v>40</v>
       </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
       <c r="C23">
         <v>45</v>
       </c>
@@ -5862,6 +6333,9 @@
       <c r="A24">
         <v>41</v>
       </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
       <c r="C24">
         <v>24</v>
       </c>
@@ -6101,6 +6575,9 @@
       <c r="A25">
         <v>42</v>
       </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
       <c r="C25">
         <v>45</v>
       </c>
@@ -6340,6 +6817,9 @@
       <c r="A26">
         <v>43</v>
       </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
       <c r="C26">
         <v>43</v>
       </c>
@@ -6579,6 +7059,9 @@
       <c r="A27">
         <v>44</v>
       </c>
+      <c r="B27" t="s">
+        <v>28</v>
+      </c>
       <c r="C27">
         <v>53</v>
       </c>
@@ -6818,6 +7301,9 @@
       <c r="A28">
         <v>45</v>
       </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
       <c r="C28">
         <v>57</v>
       </c>
@@ -7057,6 +7543,9 @@
       <c r="A29">
         <v>46</v>
       </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
       <c r="C29">
         <v>34</v>
       </c>
@@ -7296,6 +7785,9 @@
       <c r="A30">
         <v>47</v>
       </c>
+      <c r="B30" t="s">
+        <v>31</v>
+      </c>
       <c r="C30">
         <v>39</v>
       </c>
@@ -7535,6 +8027,9 @@
       <c r="A31">
         <v>48</v>
       </c>
+      <c r="B31" t="s">
+        <v>32</v>
+      </c>
       <c r="C31">
         <v>32</v>
       </c>
@@ -7774,6 +8269,9 @@
       <c r="A32">
         <v>49</v>
       </c>
+      <c r="B32" t="s">
+        <v>33</v>
+      </c>
       <c r="C32">
         <v>62</v>
       </c>
@@ -8013,6 +8511,9 @@
       <c r="A33">
         <v>50</v>
       </c>
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
       <c r="C33">
         <v>35</v>
       </c>
@@ -8252,6 +8753,9 @@
       <c r="A34">
         <v>51</v>
       </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
       <c r="C34">
         <v>29</v>
       </c>
@@ -8491,6 +8995,9 @@
       <c r="A35">
         <v>52</v>
       </c>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
       <c r="C35">
         <v>35</v>
       </c>
@@ -8730,6 +9237,9 @@
       <c r="A36">
         <v>53</v>
       </c>
+      <c r="B36" t="s">
+        <v>37</v>
+      </c>
       <c r="C36">
         <v>24</v>
       </c>
@@ -8969,6 +9479,9 @@
       <c r="A37">
         <v>54</v>
       </c>
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
       <c r="C37">
         <v>18</v>
       </c>
@@ -9208,6 +9721,9 @@
       <c r="A38">
         <v>55</v>
       </c>
+      <c r="B38" t="s">
+        <v>39</v>
+      </c>
       <c r="C38">
         <v>34</v>
       </c>
@@ -9447,6 +9963,9 @@
       <c r="A39">
         <v>56</v>
       </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
       <c r="C39">
         <v>27</v>
       </c>
@@ -9686,6 +10205,9 @@
       <c r="A40">
         <v>57</v>
       </c>
+      <c r="B40" t="s">
+        <v>41</v>
+      </c>
       <c r="C40">
         <v>22</v>
       </c>
@@ -9925,6 +10447,9 @@
       <c r="A41">
         <v>58</v>
       </c>
+      <c r="B41" t="s">
+        <v>42</v>
+      </c>
       <c r="C41">
         <v>34</v>
       </c>
@@ -10164,6 +10689,9 @@
       <c r="A42">
         <v>59</v>
       </c>
+      <c r="B42" t="s">
+        <v>43</v>
+      </c>
       <c r="C42">
         <v>28</v>
       </c>
@@ -10403,6 +10931,9 @@
       <c r="A43">
         <v>60</v>
       </c>
+      <c r="B43" t="s">
+        <v>44</v>
+      </c>
       <c r="C43">
         <v>18</v>
       </c>
@@ -10642,6 +11173,9 @@
       <c r="A44">
         <v>61</v>
       </c>
+      <c r="B44" t="s">
+        <v>45</v>
+      </c>
       <c r="C44">
         <v>22</v>
       </c>
@@ -11120,6 +11654,9 @@
       <c r="A46">
         <v>63</v>
       </c>
+      <c r="B46" t="s">
+        <v>46</v>
+      </c>
       <c r="C46">
         <v>17</v>
       </c>
@@ -11359,6 +11896,9 @@
       <c r="A47">
         <v>64</v>
       </c>
+      <c r="B47" t="s">
+        <v>47</v>
+      </c>
       <c r="C47">
         <v>9</v>
       </c>
@@ -11837,6 +12377,9 @@
       <c r="A49">
         <v>66</v>
       </c>
+      <c r="B49" t="s">
+        <v>48</v>
+      </c>
       <c r="C49">
         <v>28</v>
       </c>
@@ -12315,6 +12858,9 @@
       <c r="A51">
         <v>68</v>
       </c>
+      <c r="B51" t="s">
+        <v>49</v>
+      </c>
       <c r="C51">
         <v>365</v>
       </c>
@@ -12554,6 +13100,9 @@
       <c r="A52">
         <v>69</v>
       </c>
+      <c r="B52" t="s">
+        <v>50</v>
+      </c>
       <c r="C52">
         <v>13</v>
       </c>
@@ -12793,6 +13342,9 @@
       <c r="A53">
         <v>70</v>
       </c>
+      <c r="B53" t="s">
+        <v>51</v>
+      </c>
       <c r="C53">
         <v>18</v>
       </c>
@@ -13032,6 +13584,9 @@
       <c r="A54">
         <v>71</v>
       </c>
+      <c r="B54" t="s">
+        <v>52</v>
+      </c>
       <c r="C54">
         <v>16</v>
       </c>
@@ -13271,6 +13826,9 @@
       <c r="A55">
         <v>72</v>
       </c>
+      <c r="B55" t="s">
+        <v>53</v>
+      </c>
       <c r="C55">
         <v>6</v>
       </c>
@@ -13510,6 +14068,9 @@
       <c r="A56">
         <v>73</v>
       </c>
+      <c r="B56" t="s">
+        <v>54</v>
+      </c>
       <c r="C56">
         <v>9</v>
       </c>
@@ -13749,6 +14310,9 @@
       <c r="A57">
         <v>74</v>
       </c>
+      <c r="B57" t="s">
+        <v>55</v>
+      </c>
       <c r="C57">
         <v>12</v>
       </c>
@@ -13988,6 +14552,9 @@
       <c r="A58">
         <v>75</v>
       </c>
+      <c r="B58" t="s">
+        <v>56</v>
+      </c>
       <c r="C58">
         <v>14</v>
       </c>
@@ -14705,6 +15272,9 @@
       <c r="A61">
         <v>79</v>
       </c>
+      <c r="B61" t="s">
+        <v>57</v>
+      </c>
       <c r="C61">
         <v>13</v>
       </c>
@@ -14944,6 +15514,9 @@
       <c r="A62">
         <v>80</v>
       </c>
+      <c r="B62" t="s">
+        <v>58</v>
+      </c>
       <c r="C62">
         <v>10</v>
       </c>
@@ -15183,6 +15756,9 @@
       <c r="A63">
         <v>81</v>
       </c>
+      <c r="B63" t="s">
+        <v>59</v>
+      </c>
       <c r="C63">
         <v>66</v>
       </c>
@@ -15422,6 +15998,9 @@
       <c r="A64">
         <v>83</v>
       </c>
+      <c r="B64" t="s">
+        <v>60</v>
+      </c>
       <c r="C64">
         <v>4</v>
       </c>
@@ -15661,6 +16240,9 @@
       <c r="A65">
         <v>84</v>
       </c>
+      <c r="B65" t="s">
+        <v>61</v>
+      </c>
       <c r="C65">
         <v>11</v>
       </c>
@@ -15900,6 +16482,9 @@
       <c r="A66">
         <v>86</v>
       </c>
+      <c r="B66" t="s">
+        <v>62</v>
+      </c>
       <c r="C66">
         <v>6</v>
       </c>
@@ -16139,6 +16724,9 @@
       <c r="A67">
         <v>87</v>
       </c>
+      <c r="B67" t="s">
+        <v>63</v>
+      </c>
       <c r="C67">
         <v>8</v>
       </c>
@@ -16378,6 +16966,9 @@
       <c r="A68">
         <v>88</v>
       </c>
+      <c r="B68" t="s">
+        <v>64</v>
+      </c>
       <c r="C68">
         <v>5</v>
       </c>
@@ -16617,6 +17208,9 @@
       <c r="A69">
         <v>89</v>
       </c>
+      <c r="B69" t="s">
+        <v>65</v>
+      </c>
       <c r="C69">
         <v>10</v>
       </c>
@@ -16856,6 +17450,9 @@
       <c r="A70">
         <v>90</v>
       </c>
+      <c r="B70" t="s">
+        <v>66</v>
+      </c>
       <c r="C70">
         <v>9</v>
       </c>
@@ -17095,6 +17692,9 @@
       <c r="A71">
         <v>91</v>
       </c>
+      <c r="B71" t="s">
+        <v>67</v>
+      </c>
       <c r="C71">
         <v>31</v>
       </c>
@@ -17334,6 +17934,9 @@
       <c r="A72">
         <v>92</v>
       </c>
+      <c r="B72" t="s">
+        <v>68</v>
+      </c>
       <c r="C72">
         <v>5</v>
       </c>
@@ -17573,6 +18176,9 @@
       <c r="A73">
         <v>94</v>
       </c>
+      <c r="B73" t="s">
+        <v>69</v>
+      </c>
       <c r="C73">
         <v>5</v>
       </c>
@@ -17812,6 +18418,9 @@
       <c r="A74">
         <v>95</v>
       </c>
+      <c r="B74" t="s">
+        <v>70</v>
+      </c>
       <c r="C74">
         <v>13</v>
       </c>
@@ -18051,6 +18660,9 @@
       <c r="A75">
         <v>96</v>
       </c>
+      <c r="B75" t="s">
+        <v>71</v>
+      </c>
       <c r="C75">
         <v>14</v>
       </c>
@@ -18290,6 +18902,9 @@
       <c r="A76">
         <v>98</v>
       </c>
+      <c r="B76" t="s">
+        <v>72</v>
+      </c>
       <c r="C76">
         <v>4</v>
       </c>
@@ -18529,6 +19144,9 @@
       <c r="A77">
         <v>99</v>
       </c>
+      <c r="B77" t="s">
+        <v>73</v>
+      </c>
       <c r="C77">
         <v>11</v>
       </c>
@@ -18768,6 +19386,9 @@
       <c r="A78">
         <v>100</v>
       </c>
+      <c r="B78" t="s">
+        <v>74</v>
+      </c>
       <c r="C78">
         <v>3</v>
       </c>
@@ -19963,6 +20584,9 @@
       <c r="A83">
         <v>114</v>
       </c>
+      <c r="B83" t="s">
+        <v>75</v>
+      </c>
       <c r="C83">
         <v>8</v>
       </c>
@@ -21158,6 +21782,9 @@
       <c r="A88">
         <v>120</v>
       </c>
+      <c r="B88" t="s">
+        <v>76</v>
+      </c>
       <c r="C88">
         <v>4</v>
       </c>
@@ -21397,6 +22024,9 @@
       <c r="A89">
         <v>122</v>
       </c>
+      <c r="B89" t="s">
+        <v>77</v>
+      </c>
       <c r="C89">
         <v>7</v>
       </c>
@@ -21636,6 +22266,9 @@
       <c r="A90">
         <v>123</v>
       </c>
+      <c r="B90" t="s">
+        <v>78</v>
+      </c>
       <c r="C90">
         <v>52</v>
       </c>
@@ -21875,6 +22508,9 @@
       <c r="A91">
         <v>124</v>
       </c>
+      <c r="B91" t="s">
+        <v>79</v>
+      </c>
       <c r="C91">
         <v>5</v>
       </c>
@@ -22114,6 +22750,9 @@
       <c r="A92">
         <v>128</v>
       </c>
+      <c r="B92" t="s">
+        <v>80</v>
+      </c>
       <c r="C92">
         <v>15</v>
       </c>
@@ -22353,6 +22992,9 @@
       <c r="A93">
         <v>130</v>
       </c>
+      <c r="B93" t="s">
+        <v>81</v>
+      </c>
       <c r="C93">
         <v>8</v>
       </c>
@@ -23070,6 +23712,9 @@
       <c r="A96">
         <v>135</v>
       </c>
+      <c r="B96" t="s">
+        <v>82</v>
+      </c>
       <c r="C96">
         <v>21</v>
       </c>
@@ -23548,6 +24193,9 @@
       <c r="A98">
         <v>137</v>
       </c>
+      <c r="B98" t="s">
+        <v>83</v>
+      </c>
       <c r="C98">
         <v>3</v>
       </c>
@@ -24026,6 +24674,9 @@
       <c r="A100">
         <v>140</v>
       </c>
+      <c r="B100" t="s">
+        <v>84</v>
+      </c>
       <c r="C100">
         <v>65</v>
       </c>
@@ -24265,6 +24916,9 @@
       <c r="A101">
         <v>141</v>
       </c>
+      <c r="B101" t="s">
+        <v>85</v>
+      </c>
       <c r="C101">
         <v>4</v>
       </c>
@@ -24504,6 +25158,9 @@
       <c r="A102">
         <v>142</v>
       </c>
+      <c r="B102" t="s">
+        <v>86</v>
+      </c>
       <c r="C102">
         <v>3</v>
       </c>
@@ -24743,6 +25400,9 @@
       <c r="A103">
         <v>143</v>
       </c>
+      <c r="B103" t="s">
+        <v>87</v>
+      </c>
       <c r="C103">
         <v>17</v>
       </c>
@@ -24982,6 +25642,9 @@
       <c r="A104">
         <v>145</v>
       </c>
+      <c r="B104" t="s">
+        <v>88</v>
+      </c>
       <c r="C104">
         <v>5</v>
       </c>
@@ -25221,6 +25884,9 @@
       <c r="A105">
         <v>146</v>
       </c>
+      <c r="B105" t="s">
+        <v>89</v>
+      </c>
       <c r="C105">
         <v>7</v>
       </c>
@@ -25460,6 +26126,9 @@
       <c r="A106">
         <v>150</v>
       </c>
+      <c r="B106" t="s">
+        <v>90</v>
+      </c>
       <c r="C106">
         <v>6</v>
       </c>
@@ -25699,6 +26368,9 @@
       <c r="A107">
         <v>154</v>
       </c>
+      <c r="B107" t="s">
+        <v>91</v>
+      </c>
       <c r="C107">
         <v>8</v>
       </c>
@@ -27850,6 +28522,9 @@
       <c r="A116">
         <v>180</v>
       </c>
+      <c r="B116" t="s">
+        <v>92</v>
+      </c>
       <c r="C116">
         <v>25</v>
       </c>
@@ -28089,6 +28764,9 @@
       <c r="A117">
         <v>181</v>
       </c>
+      <c r="B117" t="s">
+        <v>93</v>
+      </c>
       <c r="C117">
         <v>20</v>
       </c>
@@ -28328,6 +29006,9 @@
       <c r="A118">
         <v>184</v>
       </c>
+      <c r="B118" t="s">
+        <v>94</v>
+      </c>
       <c r="C118">
         <v>76</v>
       </c>
@@ -28567,6 +29248,9 @@
       <c r="A119">
         <v>186</v>
       </c>
+      <c r="B119" t="s">
+        <v>95</v>
+      </c>
       <c r="C119">
         <v>4</v>
       </c>
@@ -28806,6 +29490,9 @@
       <c r="A120">
         <v>187</v>
       </c>
+      <c r="B120" t="s">
+        <v>96</v>
+      </c>
       <c r="C120">
         <v>6</v>
       </c>
@@ -29045,6 +29732,9 @@
       <c r="A121">
         <v>189</v>
       </c>
+      <c r="B121" t="s">
+        <v>97</v>
+      </c>
       <c r="C121">
         <v>161</v>
       </c>
@@ -29284,6 +29974,9 @@
       <c r="A122">
         <v>190</v>
       </c>
+      <c r="B122" t="s">
+        <v>98</v>
+      </c>
       <c r="C122">
         <v>4</v>
       </c>
@@ -29523,6 +30216,9 @@
       <c r="A123">
         <v>192</v>
       </c>
+      <c r="B123" t="s">
+        <v>99</v>
+      </c>
       <c r="C123">
         <v>10</v>
       </c>
@@ -29762,6 +30458,9 @@
       <c r="A124">
         <v>194</v>
       </c>
+      <c r="B124" t="s">
+        <v>100</v>
+      </c>
       <c r="C124">
         <v>65</v>
       </c>
@@ -30001,6 +30700,9 @@
       <c r="A125">
         <v>195</v>
       </c>
+      <c r="B125" t="s">
+        <v>101</v>
+      </c>
       <c r="C125">
         <v>4</v>
       </c>
@@ -30240,6 +30942,9 @@
       <c r="A126">
         <v>197</v>
       </c>
+      <c r="B126" t="s">
+        <v>102</v>
+      </c>
       <c r="C126">
         <v>3</v>
       </c>
@@ -30479,6 +31184,9 @@
       <c r="A127">
         <v>198</v>
       </c>
+      <c r="B127" t="s">
+        <v>103</v>
+      </c>
       <c r="C127">
         <v>5</v>
       </c>
@@ -30718,6 +31426,9 @@
       <c r="A128">
         <v>199</v>
       </c>
+      <c r="B128" t="s">
+        <v>104</v>
+      </c>
       <c r="C128">
         <v>16</v>
       </c>
@@ -30957,6 +31668,9 @@
       <c r="A129">
         <v>201</v>
       </c>
+      <c r="B129" t="s">
+        <v>105</v>
+      </c>
       <c r="C129">
         <v>122</v>
       </c>
@@ -31196,6 +31910,9 @@
       <c r="A130">
         <v>202</v>
       </c>
+      <c r="B130" t="s">
+        <v>106</v>
+      </c>
       <c r="C130">
         <v>42</v>
       </c>
@@ -31435,6 +32152,9 @@
       <c r="A131">
         <v>203</v>
       </c>
+      <c r="B131" t="s">
+        <v>107</v>
+      </c>
       <c r="C131">
         <v>20</v>
       </c>
@@ -31674,6 +32394,9 @@
       <c r="A132">
         <v>204</v>
       </c>
+      <c r="B132" t="s">
+        <v>108</v>
+      </c>
       <c r="C132">
         <v>3</v>
       </c>
@@ -31913,6 +32636,9 @@
       <c r="A133">
         <v>205</v>
       </c>
+      <c r="B133" t="s">
+        <v>109</v>
+      </c>
       <c r="C133">
         <v>50</v>
       </c>
@@ -32152,6 +32878,9 @@
       <c r="A134">
         <v>208</v>
       </c>
+      <c r="B134" t="s">
+        <v>110</v>
+      </c>
       <c r="C134">
         <v>9</v>
       </c>
@@ -32391,6 +33120,9 @@
       <c r="A135">
         <v>209</v>
       </c>
+      <c r="B135" t="s">
+        <v>111</v>
+      </c>
       <c r="C135">
         <v>8</v>
       </c>
@@ -32630,6 +33362,9 @@
       <c r="A136">
         <v>214</v>
       </c>
+      <c r="B136" t="s">
+        <v>112</v>
+      </c>
       <c r="C136">
         <v>101</v>
       </c>
@@ -32869,6 +33604,9 @@
       <c r="A137">
         <v>215</v>
       </c>
+      <c r="B137" t="s">
+        <v>113</v>
+      </c>
       <c r="C137">
         <v>4</v>
       </c>
@@ -33108,6 +33846,9 @@
       <c r="A138">
         <v>216</v>
       </c>
+      <c r="B138" t="s">
+        <v>114</v>
+      </c>
       <c r="C138">
         <v>10</v>
       </c>
@@ -33347,6 +34088,9 @@
       <c r="A139">
         <v>220</v>
       </c>
+      <c r="B139" t="s">
+        <v>115</v>
+      </c>
       <c r="C139">
         <v>14</v>
       </c>
@@ -33586,6 +34330,9 @@
       <c r="A140">
         <v>222</v>
       </c>
+      <c r="B140" t="s">
+        <v>116</v>
+      </c>
       <c r="C140">
         <v>3</v>
       </c>
@@ -33825,6 +34572,9 @@
       <c r="A141">
         <v>224</v>
       </c>
+      <c r="B141" t="s">
+        <v>117</v>
+      </c>
       <c r="C141">
         <v>4</v>
       </c>
@@ -34064,6 +34814,9 @@
       <c r="A142">
         <v>235</v>
       </c>
+      <c r="B142" t="s">
+        <v>118</v>
+      </c>
       <c r="C142">
         <v>10</v>
       </c>
@@ -34303,6 +35056,9 @@
       <c r="A143">
         <v>237</v>
       </c>
+      <c r="B143" t="s">
+        <v>119</v>
+      </c>
       <c r="C143">
         <v>44</v>
       </c>
@@ -34542,6 +35298,9 @@
       <c r="A144">
         <v>238</v>
       </c>
+      <c r="B144" t="s">
+        <v>120</v>
+      </c>
       <c r="C144">
         <v>12</v>
       </c>
@@ -34781,6 +35540,9 @@
       <c r="A145">
         <v>245</v>
       </c>
+      <c r="B145" t="s">
+        <v>121</v>
+      </c>
       <c r="C145">
         <v>71</v>
       </c>
@@ -35020,6 +35782,9 @@
       <c r="A146">
         <v>246</v>
       </c>
+      <c r="B146" t="s">
+        <v>122</v>
+      </c>
       <c r="C146">
         <v>9</v>
       </c>
@@ -35259,6 +36024,9 @@
       <c r="A147">
         <v>247</v>
       </c>
+      <c r="B147" t="s">
+        <v>123</v>
+      </c>
       <c r="C147">
         <v>32</v>
       </c>
@@ -35498,6 +36266,9 @@
       <c r="A148">
         <v>248</v>
       </c>
+      <c r="B148" t="s">
+        <v>124</v>
+      </c>
       <c r="C148">
         <v>4</v>
       </c>
@@ -35737,6 +36508,9 @@
       <c r="A149">
         <v>249</v>
       </c>
+      <c r="B149" t="s">
+        <v>125</v>
+      </c>
       <c r="C149">
         <v>64</v>
       </c>
@@ -35976,6 +36750,9 @@
       <c r="A150">
         <v>251</v>
       </c>
+      <c r="B150" t="s">
+        <v>126</v>
+      </c>
       <c r="C150">
         <v>5</v>
       </c>
@@ -36215,6 +36992,9 @@
       <c r="A151">
         <v>252</v>
       </c>
+      <c r="B151" t="s">
+        <v>127</v>
+      </c>
       <c r="C151">
         <v>65</v>
       </c>
@@ -36454,6 +37234,9 @@
       <c r="A152">
         <v>253</v>
       </c>
+      <c r="B152" t="s">
+        <v>128</v>
+      </c>
       <c r="C152">
         <v>9</v>
       </c>
@@ -36693,6 +37476,9 @@
       <c r="A153">
         <v>254</v>
       </c>
+      <c r="B153" t="s">
+        <v>129</v>
+      </c>
       <c r="C153">
         <v>125</v>
       </c>
@@ -36932,6 +37718,9 @@
       <c r="A154">
         <v>255</v>
       </c>
+      <c r="B154" t="s">
+        <v>130</v>
+      </c>
       <c r="C154">
         <v>4</v>
       </c>
@@ -37171,6 +37960,9 @@
       <c r="A155">
         <v>258</v>
       </c>
+      <c r="B155" t="s">
+        <v>131</v>
+      </c>
       <c r="C155">
         <v>19</v>
       </c>
@@ -37410,6 +38202,9 @@
       <c r="A156">
         <v>259</v>
       </c>
+      <c r="B156" t="s">
+        <v>132</v>
+      </c>
       <c r="C156">
         <v>26</v>
       </c>
@@ -37649,6 +38444,9 @@
       <c r="A157">
         <v>269</v>
       </c>
+      <c r="B157" t="s">
+        <v>133</v>
+      </c>
       <c r="C157">
         <v>11</v>
       </c>
@@ -37888,6 +38686,9 @@
       <c r="A158">
         <v>270</v>
       </c>
+      <c r="B158" t="s">
+        <v>134</v>
+      </c>
       <c r="C158">
         <v>8</v>
       </c>
@@ -38127,6 +38928,9 @@
       <c r="A159">
         <v>271</v>
       </c>
+      <c r="B159" t="s">
+        <v>135</v>
+      </c>
       <c r="C159">
         <v>19</v>
       </c>
@@ -38366,6 +39170,9 @@
       <c r="A160">
         <v>272</v>
       </c>
+      <c r="B160" t="s">
+        <v>136</v>
+      </c>
       <c r="C160">
         <v>45</v>
       </c>
@@ -38604,6 +39411,9 @@
     <row r="161" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>275</v>
+      </c>
+      <c r="B161" t="s">
+        <v>137</v>
       </c>
       <c r="C161">
         <v>50</v>

</xml_diff>

<commit_message>
Completed all legible tree species names
</commit_message>
<xml_diff>
--- a/Lovejoy_data_table_tree_frequency.xlsx
+++ b/Lovejoy_data_table_tree_frequency.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="215">
   <si>
     <t>Treespecies</t>
   </si>
@@ -439,6 +439,237 @@
   <si>
     <t>Vochysia Guianensis</t>
   </si>
+  <si>
+    <t>Vouacapoua Americana</t>
+  </si>
+  <si>
+    <t>Eschweilera Amara</t>
+  </si>
+  <si>
+    <t>Taralea Oppositifolia</t>
+  </si>
+  <si>
+    <t>Tapirira Guianensis</t>
+  </si>
+  <si>
+    <t>Eschweilera Fracia</t>
+  </si>
+  <si>
+    <t>Mauritiella sp.</t>
+  </si>
+  <si>
+    <t>Diospyros Guianensis</t>
+  </si>
+  <si>
+    <t>Bombax Aquaticum</t>
+  </si>
+  <si>
+    <t>Ambelania Grandiflora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calyptranthes Cuspidata </t>
+  </si>
+  <si>
+    <t>Socratea Exorrhiza</t>
+  </si>
+  <si>
+    <t>Alchorneopsis Trimera</t>
+  </si>
+  <si>
+    <t>Ficus Pulchella</t>
+  </si>
+  <si>
+    <t>Caraipa sp.</t>
+  </si>
+  <si>
+    <t>Pourouma Paraensis</t>
+  </si>
+  <si>
+    <t>Tapirira sp.</t>
+  </si>
+  <si>
+    <t>Piptadenia sp.</t>
+  </si>
+  <si>
+    <t>Conceveiba sp.</t>
+  </si>
+  <si>
+    <t>Xylopia sp.</t>
+  </si>
+  <si>
+    <t>Theobroma sp.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parkia Multyjuga </t>
+  </si>
+  <si>
+    <t>Hieronyma sp.</t>
+  </si>
+  <si>
+    <t>Mora Paraensis</t>
+  </si>
+  <si>
+    <t>Xylopia Nitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Socratea sp. </t>
+  </si>
+  <si>
+    <t>Rinorea Guianensis</t>
+  </si>
+  <si>
+    <t>Tachigalia sp.</t>
+  </si>
+  <si>
+    <t>Rinorea sp.</t>
+  </si>
+  <si>
+    <t>Guarea sp.</t>
+  </si>
+  <si>
+    <t>Jacaranda Copaia</t>
+  </si>
+  <si>
+    <t>Licania Canescens</t>
+  </si>
+  <si>
+    <t>Inga Grandifolia</t>
+  </si>
+  <si>
+    <t>Eronema sp.</t>
+  </si>
+  <si>
+    <t>Rheedia Floribunda</t>
+  </si>
+  <si>
+    <t>Sapium Mamieri</t>
+  </si>
+  <si>
+    <t>Eugenia Feijoi</t>
+  </si>
+  <si>
+    <t>Macrolobium Pendulum</t>
+  </si>
+  <si>
+    <t>Stericulia sp.</t>
+  </si>
+  <si>
+    <t>Terminalia Guianensis</t>
+  </si>
+  <si>
+    <t>Maximilia Regia</t>
+  </si>
+  <si>
+    <t>Swartzia Acuminata</t>
+  </si>
+  <si>
+    <t>Cordia Exaltata</t>
+  </si>
+  <si>
+    <t>Inga Gracifolia</t>
+  </si>
+  <si>
+    <t>Combretum Coconcia</t>
+  </si>
+  <si>
+    <t>Tapura sp.</t>
+  </si>
+  <si>
+    <t>Ormosia Continhoi</t>
+  </si>
+  <si>
+    <t>Quararibea Guianensis</t>
+  </si>
+  <si>
+    <t>Astrocaryum Murumuru</t>
+  </si>
+  <si>
+    <t>Crudia sp.</t>
+  </si>
+  <si>
+    <t>Theobroma Cacau</t>
+  </si>
+  <si>
+    <t>Phecolobre</t>
+  </si>
+  <si>
+    <t>Fagara Rhoifolia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virma </t>
+  </si>
+  <si>
+    <t>Byrsonima Amazonica</t>
+  </si>
+  <si>
+    <t>Eschweilera Amazonica</t>
+  </si>
+  <si>
+    <t>Himatanthus Sucunba</t>
+  </si>
+  <si>
+    <t>Ormosia sp.</t>
+  </si>
+  <si>
+    <t>Miconia Minutifolia</t>
+  </si>
+  <si>
+    <t>Bagassa Guianensis</t>
+  </si>
+  <si>
+    <t>Laetia sp.</t>
+  </si>
+  <si>
+    <t>Parkia sp.</t>
+  </si>
+  <si>
+    <t>Moracea sp.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crudia Bifolia </t>
+  </si>
+  <si>
+    <t>Licania Leniata</t>
+  </si>
+  <si>
+    <t>Melastomacia</t>
+  </si>
+  <si>
+    <t>Lauracea sp.</t>
+  </si>
+  <si>
+    <t>Triplaris Martiana</t>
+  </si>
+  <si>
+    <t>Xylopia Aromatica</t>
+  </si>
+  <si>
+    <t>Taralea Bifolia</t>
+  </si>
+  <si>
+    <t>Qualea Bifolia</t>
+  </si>
+  <si>
+    <t>Macrolobium sp.</t>
+  </si>
+  <si>
+    <t>Endopleura Uchi</t>
+  </si>
+  <si>
+    <t>Goupia sp.</t>
+  </si>
+  <si>
+    <t>Vantanea sp.</t>
+  </si>
+  <si>
+    <t>Inga Cicifolia</t>
+  </si>
+  <si>
+    <t>Labatia Macrocarpo</t>
+  </si>
+  <si>
+    <t>Licania Mahuba</t>
+  </si>
 </sst>
 </file>
 
@@ -757,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CB250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A234" workbookViewId="0">
-      <selection activeCell="B162" sqref="B162"/>
+    <sheetView tabSelected="1" topLeftCell="A224" workbookViewId="0">
+      <selection activeCell="D252" sqref="D252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39654,6 +39885,9 @@
       <c r="A162">
         <v>277</v>
       </c>
+      <c r="B162" t="s">
+        <v>138</v>
+      </c>
       <c r="C162">
         <v>51</v>
       </c>
@@ -39893,6 +40127,9 @@
       <c r="A163">
         <v>290</v>
       </c>
+      <c r="B163" t="s">
+        <v>142</v>
+      </c>
       <c r="C163">
         <v>26</v>
       </c>
@@ -40132,6 +40369,9 @@
       <c r="A164">
         <v>292</v>
       </c>
+      <c r="B164" t="s">
+        <v>140</v>
+      </c>
       <c r="C164">
         <v>39</v>
       </c>
@@ -40371,6 +40611,9 @@
       <c r="A165">
         <v>294</v>
       </c>
+      <c r="B165" t="s">
+        <v>141</v>
+      </c>
       <c r="C165">
         <v>127</v>
       </c>
@@ -40610,6 +40853,9 @@
       <c r="A166">
         <v>298</v>
       </c>
+      <c r="B166" t="s">
+        <v>139</v>
+      </c>
       <c r="C166">
         <v>90</v>
       </c>
@@ -40849,6 +41095,9 @@
       <c r="A167">
         <v>302</v>
       </c>
+      <c r="B167" t="s">
+        <v>143</v>
+      </c>
       <c r="C167">
         <v>5</v>
       </c>
@@ -41088,6 +41337,9 @@
       <c r="A168">
         <v>303</v>
       </c>
+      <c r="B168" t="s">
+        <v>144</v>
+      </c>
       <c r="C168">
         <v>8</v>
       </c>
@@ -41327,6 +41579,9 @@
       <c r="A169">
         <v>304</v>
       </c>
+      <c r="B169" t="s">
+        <v>145</v>
+      </c>
       <c r="C169">
         <v>20</v>
       </c>
@@ -41805,6 +42060,9 @@
       <c r="A171">
         <v>306</v>
       </c>
+      <c r="B171" t="s">
+        <v>146</v>
+      </c>
       <c r="C171">
         <v>13</v>
       </c>
@@ -42044,6 +42302,9 @@
       <c r="A172">
         <v>309</v>
       </c>
+      <c r="B172" t="s">
+        <v>147</v>
+      </c>
       <c r="C172">
         <v>9</v>
       </c>
@@ -42283,6 +42544,9 @@
       <c r="A173">
         <v>310</v>
       </c>
+      <c r="B173" t="s">
+        <v>148</v>
+      </c>
       <c r="C173">
         <v>50</v>
       </c>
@@ -42522,6 +42786,9 @@
       <c r="A174">
         <v>311</v>
       </c>
+      <c r="B174" t="s">
+        <v>149</v>
+      </c>
       <c r="C174">
         <v>5</v>
       </c>
@@ -42761,6 +43028,9 @@
       <c r="A175">
         <v>313</v>
       </c>
+      <c r="B175" t="s">
+        <v>150</v>
+      </c>
       <c r="C175">
         <v>15</v>
       </c>
@@ -43000,6 +43270,9 @@
       <c r="A176">
         <v>315</v>
       </c>
+      <c r="B176" t="s">
+        <v>151</v>
+      </c>
       <c r="C176">
         <v>6</v>
       </c>
@@ -43239,6 +43512,9 @@
       <c r="A177">
         <v>316</v>
       </c>
+      <c r="B177" t="s">
+        <v>152</v>
+      </c>
       <c r="C177">
         <v>5</v>
       </c>
@@ -43478,6 +43754,9 @@
       <c r="A178">
         <v>317</v>
       </c>
+      <c r="B178" t="s">
+        <v>153</v>
+      </c>
       <c r="C178">
         <v>11</v>
       </c>
@@ -43717,6 +43996,9 @@
       <c r="A179">
         <v>318</v>
       </c>
+      <c r="B179" t="s">
+        <v>154</v>
+      </c>
       <c r="C179">
         <v>4</v>
       </c>
@@ -43956,6 +44238,9 @@
       <c r="A180">
         <v>319</v>
       </c>
+      <c r="B180" t="s">
+        <v>155</v>
+      </c>
       <c r="C180">
         <v>34</v>
       </c>
@@ -44195,6 +44480,9 @@
       <c r="A181">
         <v>323</v>
       </c>
+      <c r="B181" t="s">
+        <v>156</v>
+      </c>
       <c r="C181">
         <v>3</v>
       </c>
@@ -44434,6 +44722,9 @@
       <c r="A182">
         <v>326</v>
       </c>
+      <c r="B182" t="s">
+        <v>157</v>
+      </c>
       <c r="C182">
         <v>3</v>
       </c>
@@ -44673,6 +44964,9 @@
       <c r="A183">
         <v>327</v>
       </c>
+      <c r="B183" t="s">
+        <v>158</v>
+      </c>
       <c r="C183">
         <v>11</v>
       </c>
@@ -44912,6 +45206,9 @@
       <c r="A184">
         <v>328</v>
       </c>
+      <c r="B184" t="s">
+        <v>159</v>
+      </c>
       <c r="C184">
         <v>4</v>
       </c>
@@ -45151,6 +45448,9 @@
       <c r="A185">
         <v>332</v>
       </c>
+      <c r="B185" t="s">
+        <v>163</v>
+      </c>
       <c r="C185">
         <v>104</v>
       </c>
@@ -45390,6 +45690,9 @@
       <c r="A186">
         <v>336</v>
       </c>
+      <c r="B186" t="s">
+        <v>164</v>
+      </c>
       <c r="C186">
         <v>19</v>
       </c>
@@ -45629,6 +45932,9 @@
       <c r="A187">
         <v>340</v>
       </c>
+      <c r="B187" t="s">
+        <v>165</v>
+      </c>
       <c r="C187">
         <v>133</v>
       </c>
@@ -45868,6 +46174,9 @@
       <c r="A188">
         <v>346</v>
       </c>
+      <c r="B188" t="s">
+        <v>160</v>
+      </c>
       <c r="C188">
         <v>16</v>
       </c>
@@ -46107,6 +46416,9 @@
       <c r="A189">
         <v>352</v>
       </c>
+      <c r="B189" t="s">
+        <v>161</v>
+      </c>
       <c r="C189">
         <v>19</v>
       </c>
@@ -46346,6 +46658,9 @@
       <c r="A190">
         <v>353</v>
       </c>
+      <c r="B190" t="s">
+        <v>162</v>
+      </c>
       <c r="C190">
         <v>6</v>
       </c>
@@ -46585,6 +46900,9 @@
       <c r="A191">
         <v>356</v>
       </c>
+      <c r="B191" t="s">
+        <v>166</v>
+      </c>
       <c r="C191">
         <v>7</v>
       </c>
@@ -46824,6 +47142,9 @@
       <c r="A192">
         <v>363</v>
       </c>
+      <c r="B192" t="s">
+        <v>167</v>
+      </c>
       <c r="C192">
         <v>4</v>
       </c>
@@ -47063,6 +47384,9 @@
       <c r="A193">
         <v>366</v>
       </c>
+      <c r="B193" t="s">
+        <v>168</v>
+      </c>
       <c r="C193">
         <v>102</v>
       </c>
@@ -47302,6 +47626,9 @@
       <c r="A194">
         <v>367</v>
       </c>
+      <c r="B194" t="s">
+        <v>169</v>
+      </c>
       <c r="C194">
         <v>12</v>
       </c>
@@ -47541,6 +47868,9 @@
       <c r="A195">
         <v>368</v>
       </c>
+      <c r="B195" t="s">
+        <v>170</v>
+      </c>
       <c r="C195">
         <v>87</v>
       </c>
@@ -47780,6 +48110,9 @@
       <c r="A196">
         <v>369</v>
       </c>
+      <c r="B196" t="s">
+        <v>171</v>
+      </c>
       <c r="C196">
         <v>6</v>
       </c>
@@ -48019,6 +48352,9 @@
       <c r="A197">
         <v>370</v>
       </c>
+      <c r="B197" t="s">
+        <v>172</v>
+      </c>
       <c r="C197">
         <v>8</v>
       </c>
@@ -48497,6 +48833,9 @@
       <c r="A199">
         <v>372</v>
       </c>
+      <c r="B199" t="s">
+        <v>173</v>
+      </c>
       <c r="C199">
         <v>8</v>
       </c>
@@ -48736,6 +49075,9 @@
       <c r="A200">
         <v>373</v>
       </c>
+      <c r="B200" t="s">
+        <v>174</v>
+      </c>
       <c r="C200">
         <v>48</v>
       </c>
@@ -48975,6 +49317,9 @@
       <c r="A201">
         <v>374</v>
       </c>
+      <c r="B201" t="s">
+        <v>175</v>
+      </c>
       <c r="C201">
         <v>25</v>
       </c>
@@ -49214,6 +49559,9 @@
       <c r="A202">
         <v>375</v>
       </c>
+      <c r="B202" t="s">
+        <v>177</v>
+      </c>
       <c r="C202">
         <v>10</v>
       </c>
@@ -49453,6 +49801,9 @@
       <c r="A203">
         <v>376</v>
       </c>
+      <c r="B203" t="s">
+        <v>176</v>
+      </c>
       <c r="C203">
         <v>10</v>
       </c>
@@ -49692,6 +50043,9 @@
       <c r="A204">
         <v>377</v>
       </c>
+      <c r="B204" t="s">
+        <v>178</v>
+      </c>
       <c r="C204">
         <v>12</v>
       </c>
@@ -49931,6 +50285,9 @@
       <c r="A205">
         <v>378</v>
       </c>
+      <c r="B205" t="s">
+        <v>179</v>
+      </c>
       <c r="C205">
         <v>60</v>
       </c>
@@ -50170,6 +50527,9 @@
       <c r="A206">
         <v>379</v>
       </c>
+      <c r="B206" t="s">
+        <v>180</v>
+      </c>
       <c r="C206">
         <v>216</v>
       </c>
@@ -50409,6 +50769,9 @@
       <c r="A207">
         <v>381</v>
       </c>
+      <c r="B207" t="s">
+        <v>178</v>
+      </c>
       <c r="C207">
         <v>18</v>
       </c>
@@ -50648,6 +51011,9 @@
       <c r="A208">
         <v>383</v>
       </c>
+      <c r="B208" t="s">
+        <v>181</v>
+      </c>
       <c r="C208">
         <v>4</v>
       </c>
@@ -50887,6 +51253,9 @@
       <c r="A209">
         <v>385</v>
       </c>
+      <c r="B209" t="s">
+        <v>182</v>
+      </c>
       <c r="C209">
         <v>10</v>
       </c>
@@ -51126,6 +51495,9 @@
       <c r="A210">
         <v>386</v>
       </c>
+      <c r="B210" t="s">
+        <v>183</v>
+      </c>
       <c r="C210">
         <v>8</v>
       </c>
@@ -51365,6 +51737,9 @@
       <c r="A211">
         <v>387</v>
       </c>
+      <c r="B211" t="s">
+        <v>133</v>
+      </c>
       <c r="C211">
         <v>8</v>
       </c>
@@ -51604,6 +51979,9 @@
       <c r="A212">
         <v>388</v>
       </c>
+      <c r="B212" t="s">
+        <v>184</v>
+      </c>
       <c r="C212">
         <v>28</v>
       </c>
@@ -51843,6 +52221,9 @@
       <c r="A213">
         <v>389</v>
       </c>
+      <c r="B213" t="s">
+        <v>185</v>
+      </c>
       <c r="C213">
         <v>111</v>
       </c>
@@ -52082,6 +52463,9 @@
       <c r="A214">
         <v>390</v>
       </c>
+      <c r="B214" t="s">
+        <v>186</v>
+      </c>
       <c r="C214">
         <v>21</v>
       </c>
@@ -52321,6 +52705,9 @@
       <c r="A215">
         <v>391</v>
       </c>
+      <c r="B215" t="s">
+        <v>187</v>
+      </c>
       <c r="C215">
         <v>11</v>
       </c>
@@ -52560,6 +52947,9 @@
       <c r="A216">
         <v>393</v>
       </c>
+      <c r="B216" t="s">
+        <v>188</v>
+      </c>
       <c r="C216">
         <v>9</v>
       </c>
@@ -52799,6 +53189,9 @@
       <c r="A217">
         <v>396</v>
       </c>
+      <c r="B217" t="s">
+        <v>176</v>
+      </c>
       <c r="C217">
         <v>13</v>
       </c>
@@ -53277,6 +53670,9 @@
       <c r="A219">
         <v>399</v>
       </c>
+      <c r="B219" t="s">
+        <v>189</v>
+      </c>
       <c r="C219">
         <v>6</v>
       </c>
@@ -53516,6 +53912,9 @@
       <c r="A220">
         <v>400</v>
       </c>
+      <c r="B220" t="s">
+        <v>190</v>
+      </c>
       <c r="C220">
         <v>70</v>
       </c>
@@ -53755,6 +54154,9 @@
       <c r="A221">
         <v>401</v>
       </c>
+      <c r="B221" t="s">
+        <v>191</v>
+      </c>
       <c r="C221">
         <v>3</v>
       </c>
@@ -53994,6 +54396,9 @@
       <c r="A222">
         <v>407</v>
       </c>
+      <c r="B222" t="s">
+        <v>192</v>
+      </c>
       <c r="C222">
         <v>14</v>
       </c>
@@ -54233,6 +54638,9 @@
       <c r="A223">
         <v>408</v>
       </c>
+      <c r="B223" t="s">
+        <v>193</v>
+      </c>
       <c r="C223">
         <v>6</v>
       </c>
@@ -54472,6 +54880,9 @@
       <c r="A224">
         <v>409</v>
       </c>
+      <c r="B224" t="s">
+        <v>194</v>
+      </c>
       <c r="C224">
         <v>3</v>
       </c>
@@ -54711,6 +55122,9 @@
       <c r="A225">
         <v>410</v>
       </c>
+      <c r="B225" t="s">
+        <v>195</v>
+      </c>
       <c r="C225">
         <v>12</v>
       </c>
@@ -54950,6 +55364,9 @@
       <c r="A226">
         <v>413</v>
       </c>
+      <c r="B226" t="s">
+        <v>191</v>
+      </c>
       <c r="C226">
         <v>12</v>
       </c>
@@ -55428,6 +55845,9 @@
       <c r="A228">
         <v>416</v>
       </c>
+      <c r="B228" t="s">
+        <v>196</v>
+      </c>
       <c r="C228">
         <v>3</v>
       </c>
@@ -55667,6 +56087,9 @@
       <c r="A229">
         <v>417</v>
       </c>
+      <c r="B229" t="s">
+        <v>173</v>
+      </c>
       <c r="C229">
         <v>5</v>
       </c>
@@ -55906,6 +56329,9 @@
       <c r="A230">
         <v>418</v>
       </c>
+      <c r="B230" t="s">
+        <v>204</v>
+      </c>
       <c r="C230">
         <v>8</v>
       </c>
@@ -56145,6 +56571,9 @@
       <c r="A231">
         <v>419</v>
       </c>
+      <c r="B231" t="s">
+        <v>197</v>
+      </c>
       <c r="C231">
         <v>19</v>
       </c>
@@ -56384,6 +56813,9 @@
       <c r="A232">
         <v>421</v>
       </c>
+      <c r="B232" t="s">
+        <v>198</v>
+      </c>
       <c r="C232">
         <v>4</v>
       </c>
@@ -56623,6 +57055,9 @@
       <c r="A233">
         <v>425</v>
       </c>
+      <c r="B233" t="s">
+        <v>199</v>
+      </c>
       <c r="C233">
         <v>4</v>
       </c>
@@ -56862,6 +57297,9 @@
       <c r="A234">
         <v>427</v>
       </c>
+      <c r="B234" t="s">
+        <v>200</v>
+      </c>
       <c r="C234">
         <v>8</v>
       </c>
@@ -57101,6 +57539,9 @@
       <c r="A235">
         <v>428</v>
       </c>
+      <c r="B235" t="s">
+        <v>201</v>
+      </c>
       <c r="C235">
         <v>12</v>
       </c>
@@ -57340,6 +57781,9 @@
       <c r="A236">
         <v>429</v>
       </c>
+      <c r="B236" t="s">
+        <v>202</v>
+      </c>
       <c r="C236">
         <v>15</v>
       </c>
@@ -57579,6 +58023,9 @@
       <c r="A237">
         <v>430</v>
       </c>
+      <c r="B237" t="s">
+        <v>203</v>
+      </c>
       <c r="C237">
         <v>6</v>
       </c>
@@ -57818,6 +58265,9 @@
       <c r="A238">
         <v>431</v>
       </c>
+      <c r="B238" t="s">
+        <v>205</v>
+      </c>
       <c r="C238">
         <v>4</v>
       </c>
@@ -58057,6 +58507,9 @@
       <c r="A239">
         <v>432</v>
       </c>
+      <c r="B239" t="s">
+        <v>206</v>
+      </c>
       <c r="C239">
         <v>4</v>
       </c>
@@ -58296,6 +58749,9 @@
       <c r="A240">
         <v>433</v>
       </c>
+      <c r="B240" t="s">
+        <v>207</v>
+      </c>
       <c r="C240">
         <v>3</v>
       </c>
@@ -58535,6 +58991,9 @@
       <c r="A241">
         <v>436</v>
       </c>
+      <c r="B241" t="s">
+        <v>208</v>
+      </c>
       <c r="C241">
         <v>10</v>
       </c>
@@ -59013,6 +59472,9 @@
       <c r="A243">
         <v>440</v>
       </c>
+      <c r="B243" t="s">
+        <v>209</v>
+      </c>
       <c r="C243">
         <v>5</v>
       </c>
@@ -59252,6 +59714,9 @@
       <c r="A244">
         <v>441</v>
       </c>
+      <c r="B244" t="s">
+        <v>210</v>
+      </c>
       <c r="C244">
         <v>4</v>
       </c>
@@ -59491,6 +59956,9 @@
       <c r="A245">
         <v>442</v>
       </c>
+      <c r="B245" t="s">
+        <v>211</v>
+      </c>
       <c r="C245">
         <v>6</v>
       </c>
@@ -59730,6 +60198,9 @@
       <c r="A246">
         <v>443</v>
       </c>
+      <c r="B246" t="s">
+        <v>212</v>
+      </c>
       <c r="C246">
         <v>6</v>
       </c>
@@ -59969,6 +60440,9 @@
       <c r="A247">
         <v>451</v>
       </c>
+      <c r="B247" t="s">
+        <v>184</v>
+      </c>
       <c r="C247">
         <v>32</v>
       </c>
@@ -60208,6 +60682,9 @@
       <c r="A248">
         <v>453</v>
       </c>
+      <c r="B248" t="s">
+        <v>208</v>
+      </c>
       <c r="C248">
         <v>3</v>
       </c>
@@ -60447,6 +60924,9 @@
       <c r="A249">
         <v>454</v>
       </c>
+      <c r="B249" t="s">
+        <v>213</v>
+      </c>
       <c r="C249">
         <v>3</v>
       </c>
@@ -60685,6 +61165,9 @@
     <row r="250" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>460</v>
+      </c>
+      <c r="B250" t="s">
+        <v>214</v>
       </c>
       <c r="C250">
         <v>4</v>

</xml_diff>